<commit_message>
Update data files and add new test samples
</commit_message>
<xml_diff>
--- a/data/seb.xlsx
+++ b/data/seb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matsoldin/Library/CloudStorage/Dropbox/G. AI/Projects/Budget_updater/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BA84BB-67B0-6F4B-993A-13AC9D1102E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4BA916-114F-9941-85CC-A2E1F5EBC42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
   <si>
     <t>Bokföringsdatum</t>
   </si>
@@ -45,373 +45,13 @@
     <t>Saldo</t>
   </si>
   <si>
-    <t>2025-04-30</t>
-  </si>
-  <si>
-    <t>9900002100</t>
-  </si>
-  <si>
-    <t>SYNSAM</t>
-  </si>
-  <si>
-    <t>2025-04-29</t>
-  </si>
-  <si>
-    <t>5484206268</t>
-  </si>
-  <si>
-    <t>EASYPARK    /25-04-29</t>
-  </si>
-  <si>
-    <t>5490990733</t>
-  </si>
-  <si>
-    <t>ENKLA VARDAG</t>
-  </si>
-  <si>
-    <t>2025-04-28</t>
-  </si>
-  <si>
-    <t>5484174087</t>
-  </si>
-  <si>
-    <t>EASYPARK    /25-04-28</t>
-  </si>
-  <si>
-    <t>5490990000</t>
-  </si>
-  <si>
-    <t>53653319781</t>
-  </si>
-  <si>
     <t>9900000100</t>
-  </si>
-  <si>
-    <t>AVANZA BANK</t>
-  </si>
-  <si>
-    <t>2025-04-27</t>
-  </si>
-  <si>
-    <t>5484051783</t>
-  </si>
-  <si>
-    <t>EASYPARK    /25-04-27</t>
-  </si>
-  <si>
-    <t>2025-04-25</t>
-  </si>
-  <si>
-    <t>5484538201</t>
-  </si>
-  <si>
-    <t>EASYPARK    /25-04-25</t>
-  </si>
-  <si>
-    <t>5106901784</t>
-  </si>
-  <si>
-    <t>NORDEA BANK ABP, FILIAL</t>
-  </si>
-  <si>
-    <t>5101901780</t>
-  </si>
-  <si>
-    <t>SEB KORT BANK AB</t>
-  </si>
-  <si>
-    <t>5490990543</t>
-  </si>
-  <si>
-    <t>LÖN</t>
-  </si>
-  <si>
-    <t>5097901777</t>
-  </si>
-  <si>
-    <t>VERISURE SVERIGE AB</t>
-  </si>
-  <si>
-    <t>5106901785</t>
-  </si>
-  <si>
-    <t>AKADEMIKERNAS  A-KASSA</t>
-  </si>
-  <si>
-    <t>5101901781</t>
-  </si>
-  <si>
-    <t>FORTUM MARKETS AB</t>
-  </si>
-  <si>
-    <t>5101901782</t>
-  </si>
-  <si>
-    <t>VATTENFALL KUNDSERVICE A</t>
-  </si>
-  <si>
-    <t>5106901783</t>
-  </si>
-  <si>
-    <t>LEDARNA, MEDLEMSAVGIFT</t>
-  </si>
-  <si>
-    <t>5097901778</t>
-  </si>
-  <si>
-    <t>BAHNHOF</t>
-  </si>
-  <si>
-    <t>5101901779</t>
-  </si>
-  <si>
-    <t>3 (HI3G ACCESS AB)</t>
-  </si>
-  <si>
-    <t>2025-04-23</t>
   </si>
   <si>
     <t>5490990789</t>
   </si>
   <si>
-    <t>46733347909</t>
-  </si>
-  <si>
-    <t>2025-04-22</t>
-  </si>
-  <si>
-    <t>2025-04-18</t>
-  </si>
-  <si>
-    <t>5484865309</t>
-  </si>
-  <si>
-    <t>REVOLUT  759/25-04-17</t>
-  </si>
-  <si>
-    <t>2025-04-17</t>
-  </si>
-  <si>
-    <t>5490990004</t>
-  </si>
-  <si>
-    <t>LONDON PUND</t>
-  </si>
-  <si>
-    <t>2025-04-15</t>
-  </si>
-  <si>
-    <t>5484045456</t>
-  </si>
-  <si>
-    <t>NEW YORK    /25-04-13</t>
-  </si>
-  <si>
-    <t>5484483282</t>
-  </si>
-  <si>
-    <t>REVOLUT  759/25-04-15</t>
-  </si>
-  <si>
-    <t>2025-04-14</t>
-  </si>
-  <si>
-    <t>46709124792</t>
-  </si>
-  <si>
-    <t>2025-04-13</t>
-  </si>
-  <si>
-    <t>46733233097</t>
-  </si>
-  <si>
-    <t>46735755523</t>
-  </si>
-  <si>
-    <t>46733164789</t>
-  </si>
-  <si>
-    <t>46763433833</t>
-  </si>
-  <si>
-    <t>2025-04-12</t>
-  </si>
-  <si>
-    <t>2025-04-09</t>
-  </si>
-  <si>
-    <t>2025-04-08</t>
-  </si>
-  <si>
-    <t>5484172038</t>
-  </si>
-  <si>
-    <t>BROD OCH SAL/25-04-07</t>
-  </si>
-  <si>
-    <t>2025-04-07</t>
-  </si>
-  <si>
-    <t>5484498110</t>
-  </si>
-  <si>
-    <t>EASYPARK    /25-04-07</t>
-  </si>
-  <si>
-    <t>5484418170</t>
-  </si>
-  <si>
-    <t>FOREX 858   /25-04-06</t>
-  </si>
-  <si>
-    <t>5484290435</t>
-  </si>
-  <si>
-    <t>LIFE 485    /25-04-06</t>
-  </si>
-  <si>
-    <t>2025-04-02</t>
-  </si>
-  <si>
-    <t>5484633134</t>
-  </si>
-  <si>
-    <t>EASYPARK    /25-04-02</t>
-  </si>
-  <si>
-    <t>2025-04-01</t>
-  </si>
-  <si>
-    <t>9900001100</t>
-  </si>
-  <si>
-    <t>TRYGG-HANSA</t>
-  </si>
-  <si>
-    <t>2025-03-31</t>
-  </si>
-  <si>
-    <t>2025-03-30</t>
-  </si>
-  <si>
-    <t>5484464717</t>
-  </si>
-  <si>
-    <t>EASYPARK    /25-03-30</t>
-  </si>
-  <si>
-    <t>2025-03-29</t>
-  </si>
-  <si>
-    <t>5484849864</t>
-  </si>
-  <si>
-    <t>SYSTEMBOLAGE/25-03-28</t>
-  </si>
-  <si>
-    <t>2025-03-28</t>
-  </si>
-  <si>
-    <t>2025-03-26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RÄNTOR      </t>
-  </si>
-  <si>
-    <t>2025-03-25</t>
-  </si>
-  <si>
-    <t>5484427439</t>
-  </si>
-  <si>
-    <t>EASYPARK    /25-03-25</t>
-  </si>
-  <si>
-    <t>5484323638</t>
-  </si>
-  <si>
-    <t>BROD OCH SAL/25-03-24</t>
-  </si>
-  <si>
-    <t>5070901771</t>
-  </si>
-  <si>
-    <t>5077901776</t>
-  </si>
-  <si>
-    <t>5071901772</t>
-  </si>
-  <si>
-    <t>WALLEY</t>
-  </si>
-  <si>
-    <t>5076901775</t>
-  </si>
-  <si>
-    <t>5073901774</t>
-  </si>
-  <si>
-    <t>5066901768</t>
-  </si>
-  <si>
-    <t>5073901773</t>
-  </si>
-  <si>
-    <t>5066901769</t>
-  </si>
-  <si>
-    <t>5070901770</t>
-  </si>
-  <si>
-    <t>2025-03-24</t>
-  </si>
-  <si>
-    <t>2025-03-23</t>
-  </si>
-  <si>
-    <t>5484448937</t>
-  </si>
-  <si>
-    <t>REVOLUT  759/25-03-22</t>
-  </si>
-  <si>
-    <t>46733497676</t>
-  </si>
-  <si>
-    <t>2025-03-22</t>
-  </si>
-  <si>
-    <t>5484689738</t>
-  </si>
-  <si>
-    <t>REVOLUT  759/25-03-21</t>
-  </si>
-  <si>
-    <t>5484322296</t>
-  </si>
-  <si>
-    <t>BERLIN      /25-03-21</t>
-  </si>
-  <si>
-    <t>5484646179</t>
-  </si>
-  <si>
-    <t>R C BON BON /25-03-21</t>
-  </si>
-  <si>
     <t>2025-03-21</t>
-  </si>
-  <si>
-    <t>5484071530</t>
-  </si>
-  <si>
-    <t>FOREX GALLER/25-03-20</t>
-  </si>
-  <si>
-    <t>5484753940</t>
-  </si>
-  <si>
-    <t>SCANDIC GRAN/25-03-20</t>
   </si>
   <si>
     <t>5484547089</t>
@@ -838,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3689"/>
+  <dimension ref="A1:F3627"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I83" sqref="I83"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -877,70 +517,70 @@
     </row>
     <row r="2" spans="1:6" ht="15">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4">
+        <v>-132.6</v>
+      </c>
+      <c r="F2" s="4">
+        <v>20623.580000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4">
-        <v>-665</v>
-      </c>
-      <c r="F2" s="4">
-        <v>9260.1200000000008</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="4">
-        <v>-11.3</v>
+        <v>-401.42</v>
       </c>
       <c r="F3" s="4">
-        <v>9925.1200000000008</v>
+        <v>20756.18</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="4">
-        <v>-50</v>
+        <v>-132</v>
       </c>
       <c r="F4" s="4">
-        <v>9936.42</v>
+        <v>21157.599999999999</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
@@ -949,38 +589,38 @@
         <v>16</v>
       </c>
       <c r="E5" s="4">
-        <v>-42.9</v>
+        <v>-39</v>
       </c>
       <c r="F5" s="4">
-        <v>9986.42</v>
+        <v>21289.599999999999</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E6" s="4">
-        <v>-500</v>
+        <v>-212</v>
       </c>
       <c r="F6" s="4">
-        <v>10029.32</v>
+        <v>21328.6</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>19</v>
@@ -989,98 +629,98 @@
         <v>20</v>
       </c>
       <c r="E7" s="4">
-        <v>-3400</v>
+        <v>-29</v>
       </c>
       <c r="F7" s="4">
-        <v>10529.32</v>
+        <v>21540.6</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="4">
+        <v>-428.02</v>
+      </c>
+      <c r="F8" s="4">
+        <v>21569.599999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15">
+      <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="4">
-        <v>-47.92</v>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
       </c>
-      <c r="F8" s="4">
-        <v>13929.32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15">
-      <c r="A9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="4">
+        <v>-103</v>
+      </c>
+      <c r="F9" s="4">
+        <v>21997.62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="4">
-        <v>-35.299999999999997</v>
-      </c>
-      <c r="F9" s="4">
-        <v>13977.24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="4">
+        <v>-964</v>
+      </c>
+      <c r="F10" s="4">
+        <v>22100.62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15">
+      <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="4">
-        <v>-34722.07</v>
-      </c>
-      <c r="F10" s="4">
-        <v>14012.54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="4">
+        <v>29</v>
+      </c>
+      <c r="F11" s="4">
+        <v>23064.62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15">
+      <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="4">
-        <v>-26442.63</v>
-      </c>
-      <c r="F11" s="4">
-        <v>48734.61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15">
-      <c r="A12" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>31</v>
@@ -1089,1305 +729,313 @@
         <v>32</v>
       </c>
       <c r="E12" s="4">
-        <v>66405</v>
+        <v>-34.5</v>
       </c>
       <c r="F12" s="4">
-        <v>75177.240000000005</v>
+        <v>23035.62</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="E13" s="4">
-        <v>-1737</v>
+        <v>-256</v>
       </c>
       <c r="F13" s="4">
-        <v>8772.24</v>
+        <v>23070.12</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E14" s="4">
-        <v>-140</v>
+        <v>-114</v>
       </c>
       <c r="F14" s="4">
-        <v>10509.24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="4">
-        <v>-443</v>
-      </c>
-      <c r="F15" s="4">
-        <v>10649.24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15">
-      <c r="A16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="4">
-        <v>-1037.49</v>
-      </c>
-      <c r="F16" s="4">
-        <v>11092.24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15">
-      <c r="A17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="4">
-        <v>-384</v>
-      </c>
-      <c r="F17" s="4">
-        <v>12129.73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15">
-      <c r="A18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="4">
-        <v>-859</v>
-      </c>
-      <c r="F18" s="4">
-        <v>12513.73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15">
-      <c r="A19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="4">
-        <v>-465</v>
-      </c>
-      <c r="F19" s="4">
-        <v>13372.73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15">
-      <c r="A20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="4">
-        <v>165</v>
-      </c>
-      <c r="F20" s="4">
-        <v>13837.73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15">
-      <c r="A21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="4">
-        <v>-15000</v>
-      </c>
-      <c r="F21" s="4">
-        <v>13672.73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15">
-      <c r="A22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" s="4">
-        <v>15000</v>
-      </c>
-      <c r="F22" s="4">
-        <v>28672.73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15">
-      <c r="A23" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="4">
-        <v>7.69</v>
-      </c>
-      <c r="F23" s="4">
-        <v>13672.73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15">
-      <c r="A24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="4">
-        <v>-1500</v>
-      </c>
-      <c r="F24" s="4">
-        <v>13665.04</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15">
-      <c r="A25" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="4">
-        <v>173</v>
-      </c>
-      <c r="F25" s="4">
-        <v>15165.04</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15">
-      <c r="A26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E26" s="4">
-        <v>173</v>
-      </c>
-      <c r="F26" s="4">
-        <v>14992.04</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15">
-      <c r="A27" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" s="4">
-        <v>173</v>
-      </c>
-      <c r="F27" s="4">
-        <v>14819.04</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="15">
-      <c r="A28" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="E28" s="4">
-        <v>-1191</v>
-      </c>
-      <c r="F28" s="4">
-        <v>14646.04</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="15">
-      <c r="A29" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="4">
-        <v>173</v>
-      </c>
-      <c r="F29" s="4">
-        <v>15837.04</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="15">
-      <c r="A30" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="4">
-        <v>-120</v>
-      </c>
-      <c r="F30" s="4">
-        <v>15664.04</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="15">
-      <c r="A31" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E31" s="4">
-        <v>-70</v>
-      </c>
-      <c r="F31" s="4">
-        <v>15784.04</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="15">
-      <c r="A32" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E32" s="4">
-        <v>-78</v>
-      </c>
-      <c r="F32" s="4">
-        <v>15854.04</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15">
-      <c r="A33" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E33" s="4">
-        <v>-32.85</v>
-      </c>
-      <c r="F33" s="4">
-        <v>15932.04</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15">
-      <c r="A34" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E34" s="4">
-        <v>-1071.08</v>
-      </c>
-      <c r="F34" s="4">
-        <v>15964.89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15">
-      <c r="A35" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E35" s="4">
-        <v>-617</v>
-      </c>
-      <c r="F35" s="4">
-        <v>17035.97</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="15">
-      <c r="A36" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E36" s="4">
-        <v>-32.9</v>
-      </c>
-      <c r="F36" s="4">
-        <v>17652.97</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15">
-      <c r="A37" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E37" s="4">
-        <v>-871</v>
-      </c>
-      <c r="F37" s="4">
-        <v>17685.87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="15">
-      <c r="A38" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="4">
-        <v>-665</v>
-      </c>
-      <c r="F38" s="4">
-        <v>18556.87</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="15">
-      <c r="A39" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E39" s="4">
-        <v>-64.2</v>
-      </c>
-      <c r="F39" s="4">
-        <v>19221.87</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="15">
-      <c r="A40" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E40" s="4">
-        <v>-379</v>
-      </c>
-      <c r="F40" s="4">
-        <v>19286.07</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="15">
-      <c r="A41" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" s="4">
-        <v>-500</v>
-      </c>
-      <c r="F41" s="4">
-        <v>19665.07</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="15">
-      <c r="A42" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="4">
-        <v>-50</v>
-      </c>
-      <c r="F42" s="4">
-        <v>20165.07</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="15">
-      <c r="A43" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E43" s="4">
-        <v>-4900</v>
-      </c>
-      <c r="F43" s="4">
-        <v>20215.07</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="15">
-      <c r="A44" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E44" s="4">
-        <v>-3400</v>
-      </c>
-      <c r="F44" s="4">
-        <v>25115.07</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="15">
-      <c r="A45" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E45" s="4">
-        <v>-30.1</v>
-      </c>
-      <c r="F45" s="4">
-        <v>28515.07</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="15">
-      <c r="A46" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E46" s="4">
-        <v>-78</v>
-      </c>
-      <c r="F46" s="4">
-        <v>28545.17</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="15">
-      <c r="A47" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E47" s="4">
-        <v>-27278.560000000001</v>
-      </c>
-      <c r="F47" s="4">
-        <v>28623.17</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="15">
-      <c r="A48" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E48" s="4">
-        <v>55215</v>
-      </c>
-      <c r="F48" s="4">
-        <v>55901.73</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="15">
-      <c r="A49" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E49" s="4">
-        <v>-7178.87</v>
-      </c>
-      <c r="F49" s="4">
-        <v>686.73</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="15">
-      <c r="A50" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="E50" s="4">
-        <v>-2536</v>
-      </c>
-      <c r="F50" s="4">
-        <v>7865.6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="15">
-      <c r="A51" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E51" s="4">
-        <v>-140</v>
-      </c>
-      <c r="F51" s="4">
-        <v>10401.6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="15">
-      <c r="A52" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E52" s="4">
-        <v>-559</v>
-      </c>
-      <c r="F52" s="4">
-        <v>10541.6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="15">
-      <c r="A53" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E53" s="4">
-        <v>-944.7</v>
-      </c>
-      <c r="F53" s="4">
-        <v>11100.6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="15">
-      <c r="A54" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E54" s="4">
-        <v>-319</v>
-      </c>
-      <c r="F54" s="4">
-        <v>12045.3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="15">
-      <c r="A55" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E55" s="4">
-        <v>-859</v>
-      </c>
-      <c r="F55" s="4">
-        <v>12364.3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="15">
-      <c r="A56" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E56" s="4">
-        <v>-436</v>
-      </c>
-      <c r="F56" s="4">
-        <v>13223.3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="15">
-      <c r="A57" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E57" s="4">
-        <v>-1500</v>
-      </c>
-      <c r="F57" s="4">
-        <v>13659.3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="15">
-      <c r="A58" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E58" s="4">
-        <v>-159.5</v>
-      </c>
-      <c r="F58" s="4">
-        <v>15159.3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="15">
-      <c r="A59" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E59" s="4">
-        <v>-1500</v>
-      </c>
-      <c r="F59" s="4">
-        <v>15318.8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="15">
-      <c r="A60" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E60" s="4">
-        <v>-52.94</v>
-      </c>
-      <c r="F60" s="4">
-        <v>16818.8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="15">
-      <c r="A61" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E61" s="4">
-        <v>-45</v>
-      </c>
-      <c r="F61" s="4">
-        <v>16871.740000000002</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="15">
-      <c r="A62" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E62" s="4">
-        <v>-3527.84</v>
-      </c>
-      <c r="F62" s="4">
-        <v>16916.740000000002</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="15">
-      <c r="A63" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="E63" s="4">
-        <v>-179</v>
-      </c>
-      <c r="F63" s="4">
-        <v>20444.580000000002</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="15">
-      <c r="A64" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E64" s="4">
-        <v>-132.6</v>
-      </c>
-      <c r="F64" s="4">
-        <v>20623.580000000002</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="15">
-      <c r="A65" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E65" s="4">
-        <v>-401.42</v>
-      </c>
-      <c r="F65" s="4">
-        <v>20756.18</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="15">
-      <c r="A66" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E66" s="4">
-        <v>-132</v>
-      </c>
-      <c r="F66" s="4">
-        <v>21157.599999999999</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="15">
-      <c r="A67" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E67" s="4">
-        <v>-39</v>
-      </c>
-      <c r="F67" s="4">
-        <v>21289.599999999999</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="15">
-      <c r="A68" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E68" s="4">
-        <v>-212</v>
-      </c>
-      <c r="F68" s="4">
-        <v>21328.6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="15">
-      <c r="A69" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="E69" s="4">
-        <v>-29</v>
-      </c>
-      <c r="F69" s="4">
-        <v>21540.6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="15">
-      <c r="A70" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E70" s="4">
-        <v>-428.02</v>
-      </c>
-      <c r="F70" s="4">
-        <v>21569.599999999999</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="15">
-      <c r="A71" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E71" s="4">
-        <v>-103</v>
-      </c>
-      <c r="F71" s="4">
-        <v>21997.62</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="15">
-      <c r="A72" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E72" s="4">
-        <v>-964</v>
-      </c>
-      <c r="F72" s="4">
-        <v>22100.62</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="15">
-      <c r="A73" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E73" s="4">
-        <v>29</v>
-      </c>
-      <c r="F73" s="4">
-        <v>23064.62</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="15">
-      <c r="A74" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E74" s="4">
-        <v>-34.5</v>
-      </c>
-      <c r="F74" s="4">
-        <v>23035.62</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="15">
-      <c r="A75" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E75" s="4">
-        <v>-256</v>
-      </c>
-      <c r="F75" s="4">
-        <v>23070.12</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="15">
-      <c r="A76" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E76" s="4">
-        <v>-114</v>
-      </c>
-      <c r="F76" s="4">
         <v>23326.12</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15">
+    <row r="15" spans="1:6" ht="15">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="15">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="5:6" ht="15">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="5:6" ht="15">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="5:6" ht="15">
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="5:6" ht="15">
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="5:6" ht="15">
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="5:6" ht="15">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="5:6" ht="15">
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="5:6" ht="15">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="5:6" ht="15">
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="5:6" ht="15">
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="5:6" ht="15">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="5:6" ht="15">
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="5:6" ht="15">
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="5:6" ht="15">
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="5:6" ht="15">
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="5:6" ht="15">
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="5:6" ht="15">
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="5:6" ht="15">
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="5:6" ht="15">
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="5:6" ht="15">
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="5:6" ht="15">
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="5:6" ht="15">
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+    </row>
+    <row r="39" spans="5:6" ht="15">
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="5:6" ht="15">
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="5:6" ht="15">
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="5:6" ht="15">
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="5:6" ht="15">
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="5:6" ht="15">
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="5:6" ht="15">
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="5:6" ht="15">
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="47" spans="5:6" ht="15">
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+    </row>
+    <row r="48" spans="5:6" ht="15">
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+    </row>
+    <row r="49" spans="5:6" ht="15">
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="5:6" ht="15">
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="5:6" ht="15">
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="5:6" ht="15">
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" spans="5:6" ht="15">
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+    </row>
+    <row r="54" spans="5:6" ht="15">
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+    </row>
+    <row r="55" spans="5:6" ht="15">
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+    </row>
+    <row r="56" spans="5:6" ht="15">
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+    </row>
+    <row r="57" spans="5:6" ht="15">
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+    </row>
+    <row r="58" spans="5:6" ht="15">
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+    </row>
+    <row r="59" spans="5:6" ht="15">
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+    </row>
+    <row r="60" spans="5:6" ht="15">
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+    </row>
+    <row r="61" spans="5:6" ht="15">
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" spans="5:6" ht="15">
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+    </row>
+    <row r="63" spans="5:6" ht="15">
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+    </row>
+    <row r="64" spans="5:6" ht="15">
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+    </row>
+    <row r="65" spans="5:6" ht="15">
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+    </row>
+    <row r="66" spans="5:6" ht="15">
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+    </row>
+    <row r="67" spans="5:6" ht="15">
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+    </row>
+    <row r="68" spans="5:6" ht="15">
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+    </row>
+    <row r="69" spans="5:6" ht="15">
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+    </row>
+    <row r="70" spans="5:6" ht="15">
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+    </row>
+    <row r="71" spans="5:6" ht="15">
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+    </row>
+    <row r="72" spans="5:6" ht="15">
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+    </row>
+    <row r="73" spans="5:6" ht="15">
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+    </row>
+    <row r="74" spans="5:6" ht="15">
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+    </row>
+    <row r="75" spans="5:6" ht="15">
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+    </row>
+    <row r="76" spans="5:6" ht="15">
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+    </row>
+    <row r="77" spans="5:6" ht="15">
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
     </row>
-    <row r="78" spans="1:6" ht="15">
+    <row r="78" spans="5:6" ht="15">
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
     </row>
-    <row r="79" spans="1:6" ht="15">
+    <row r="79" spans="5:6" ht="15">
       <c r="E79" s="4"/>
       <c r="F79" s="4"/>
     </row>
-    <row r="80" spans="1:6" ht="15">
+    <row r="80" spans="5:6" ht="15">
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
     </row>
@@ -16578,254 +15226,6 @@
     <row r="3627" spans="5:6" ht="15">
       <c r="E3627" s="4"/>
       <c r="F3627" s="4"/>
-    </row>
-    <row r="3628" spans="5:6" ht="15">
-      <c r="E3628" s="4"/>
-      <c r="F3628" s="4"/>
-    </row>
-    <row r="3629" spans="5:6" ht="15">
-      <c r="E3629" s="4"/>
-      <c r="F3629" s="4"/>
-    </row>
-    <row r="3630" spans="5:6" ht="15">
-      <c r="E3630" s="4"/>
-      <c r="F3630" s="4"/>
-    </row>
-    <row r="3631" spans="5:6" ht="15">
-      <c r="E3631" s="4"/>
-      <c r="F3631" s="4"/>
-    </row>
-    <row r="3632" spans="5:6" ht="15">
-      <c r="E3632" s="4"/>
-      <c r="F3632" s="4"/>
-    </row>
-    <row r="3633" spans="5:6" ht="15">
-      <c r="E3633" s="4"/>
-      <c r="F3633" s="4"/>
-    </row>
-    <row r="3634" spans="5:6" ht="15">
-      <c r="E3634" s="4"/>
-      <c r="F3634" s="4"/>
-    </row>
-    <row r="3635" spans="5:6" ht="15">
-      <c r="E3635" s="4"/>
-      <c r="F3635" s="4"/>
-    </row>
-    <row r="3636" spans="5:6" ht="15">
-      <c r="E3636" s="4"/>
-      <c r="F3636" s="4"/>
-    </row>
-    <row r="3637" spans="5:6" ht="15">
-      <c r="E3637" s="4"/>
-      <c r="F3637" s="4"/>
-    </row>
-    <row r="3638" spans="5:6" ht="15">
-      <c r="E3638" s="4"/>
-      <c r="F3638" s="4"/>
-    </row>
-    <row r="3639" spans="5:6" ht="15">
-      <c r="E3639" s="4"/>
-      <c r="F3639" s="4"/>
-    </row>
-    <row r="3640" spans="5:6" ht="15">
-      <c r="E3640" s="4"/>
-      <c r="F3640" s="4"/>
-    </row>
-    <row r="3641" spans="5:6" ht="15">
-      <c r="E3641" s="4"/>
-      <c r="F3641" s="4"/>
-    </row>
-    <row r="3642" spans="5:6" ht="15">
-      <c r="E3642" s="4"/>
-      <c r="F3642" s="4"/>
-    </row>
-    <row r="3643" spans="5:6" ht="15">
-      <c r="E3643" s="4"/>
-      <c r="F3643" s="4"/>
-    </row>
-    <row r="3644" spans="5:6" ht="15">
-      <c r="E3644" s="4"/>
-      <c r="F3644" s="4"/>
-    </row>
-    <row r="3645" spans="5:6" ht="15">
-      <c r="E3645" s="4"/>
-      <c r="F3645" s="4"/>
-    </row>
-    <row r="3646" spans="5:6" ht="15">
-      <c r="E3646" s="4"/>
-      <c r="F3646" s="4"/>
-    </row>
-    <row r="3647" spans="5:6" ht="15">
-      <c r="E3647" s="4"/>
-      <c r="F3647" s="4"/>
-    </row>
-    <row r="3648" spans="5:6" ht="15">
-      <c r="E3648" s="4"/>
-      <c r="F3648" s="4"/>
-    </row>
-    <row r="3649" spans="5:6" ht="15">
-      <c r="E3649" s="4"/>
-      <c r="F3649" s="4"/>
-    </row>
-    <row r="3650" spans="5:6" ht="15">
-      <c r="E3650" s="4"/>
-      <c r="F3650" s="4"/>
-    </row>
-    <row r="3651" spans="5:6" ht="15">
-      <c r="E3651" s="4"/>
-      <c r="F3651" s="4"/>
-    </row>
-    <row r="3652" spans="5:6" ht="15">
-      <c r="E3652" s="4"/>
-      <c r="F3652" s="4"/>
-    </row>
-    <row r="3653" spans="5:6" ht="15">
-      <c r="E3653" s="4"/>
-      <c r="F3653" s="4"/>
-    </row>
-    <row r="3654" spans="5:6" ht="15">
-      <c r="E3654" s="4"/>
-      <c r="F3654" s="4"/>
-    </row>
-    <row r="3655" spans="5:6" ht="15">
-      <c r="E3655" s="4"/>
-      <c r="F3655" s="4"/>
-    </row>
-    <row r="3656" spans="5:6" ht="15">
-      <c r="E3656" s="4"/>
-      <c r="F3656" s="4"/>
-    </row>
-    <row r="3657" spans="5:6" ht="15">
-      <c r="E3657" s="4"/>
-      <c r="F3657" s="4"/>
-    </row>
-    <row r="3658" spans="5:6" ht="15">
-      <c r="E3658" s="4"/>
-      <c r="F3658" s="4"/>
-    </row>
-    <row r="3659" spans="5:6" ht="15">
-      <c r="E3659" s="4"/>
-      <c r="F3659" s="4"/>
-    </row>
-    <row r="3660" spans="5:6" ht="15">
-      <c r="E3660" s="4"/>
-      <c r="F3660" s="4"/>
-    </row>
-    <row r="3661" spans="5:6" ht="15">
-      <c r="E3661" s="4"/>
-      <c r="F3661" s="4"/>
-    </row>
-    <row r="3662" spans="5:6" ht="15">
-      <c r="E3662" s="4"/>
-      <c r="F3662" s="4"/>
-    </row>
-    <row r="3663" spans="5:6" ht="15">
-      <c r="E3663" s="4"/>
-      <c r="F3663" s="4"/>
-    </row>
-    <row r="3664" spans="5:6" ht="15">
-      <c r="E3664" s="4"/>
-      <c r="F3664" s="4"/>
-    </row>
-    <row r="3665" spans="5:6" ht="15">
-      <c r="E3665" s="4"/>
-      <c r="F3665" s="4"/>
-    </row>
-    <row r="3666" spans="5:6" ht="15">
-      <c r="E3666" s="4"/>
-      <c r="F3666" s="4"/>
-    </row>
-    <row r="3667" spans="5:6" ht="15">
-      <c r="E3667" s="4"/>
-      <c r="F3667" s="4"/>
-    </row>
-    <row r="3668" spans="5:6" ht="15">
-      <c r="E3668" s="4"/>
-      <c r="F3668" s="4"/>
-    </row>
-    <row r="3669" spans="5:6" ht="15">
-      <c r="E3669" s="4"/>
-      <c r="F3669" s="4"/>
-    </row>
-    <row r="3670" spans="5:6" ht="15">
-      <c r="E3670" s="4"/>
-      <c r="F3670" s="4"/>
-    </row>
-    <row r="3671" spans="5:6" ht="15">
-      <c r="E3671" s="4"/>
-      <c r="F3671" s="4"/>
-    </row>
-    <row r="3672" spans="5:6" ht="15">
-      <c r="E3672" s="4"/>
-      <c r="F3672" s="4"/>
-    </row>
-    <row r="3673" spans="5:6" ht="15">
-      <c r="E3673" s="4"/>
-      <c r="F3673" s="4"/>
-    </row>
-    <row r="3674" spans="5:6" ht="15">
-      <c r="E3674" s="4"/>
-      <c r="F3674" s="4"/>
-    </row>
-    <row r="3675" spans="5:6" ht="15">
-      <c r="E3675" s="4"/>
-      <c r="F3675" s="4"/>
-    </row>
-    <row r="3676" spans="5:6" ht="15">
-      <c r="E3676" s="4"/>
-      <c r="F3676" s="4"/>
-    </row>
-    <row r="3677" spans="5:6" ht="15">
-      <c r="E3677" s="4"/>
-      <c r="F3677" s="4"/>
-    </row>
-    <row r="3678" spans="5:6" ht="15">
-      <c r="E3678" s="4"/>
-      <c r="F3678" s="4"/>
-    </row>
-    <row r="3679" spans="5:6" ht="15">
-      <c r="E3679" s="4"/>
-      <c r="F3679" s="4"/>
-    </row>
-    <row r="3680" spans="5:6" ht="15">
-      <c r="E3680" s="4"/>
-      <c r="F3680" s="4"/>
-    </row>
-    <row r="3681" spans="5:6" ht="15">
-      <c r="E3681" s="4"/>
-      <c r="F3681" s="4"/>
-    </row>
-    <row r="3682" spans="5:6" ht="15">
-      <c r="E3682" s="4"/>
-      <c r="F3682" s="4"/>
-    </row>
-    <row r="3683" spans="5:6" ht="15">
-      <c r="E3683" s="4"/>
-      <c r="F3683" s="4"/>
-    </row>
-    <row r="3684" spans="5:6" ht="15">
-      <c r="E3684" s="4"/>
-      <c r="F3684" s="4"/>
-    </row>
-    <row r="3685" spans="5:6" ht="15">
-      <c r="E3685" s="4"/>
-      <c r="F3685" s="4"/>
-    </row>
-    <row r="3686" spans="5:6" ht="15">
-      <c r="E3686" s="4"/>
-      <c r="F3686" s="4"/>
-    </row>
-    <row r="3687" spans="5:6" ht="15">
-      <c r="E3687" s="4"/>
-      <c r="F3687" s="4"/>
-    </row>
-    <row r="3688" spans="5:6" ht="15">
-      <c r="E3688" s="4"/>
-      <c r="F3688" s="4"/>
-    </row>
-    <row r="3689" spans="5:6" ht="15">
-      <c r="E3689" s="4"/>
-      <c r="F3689" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>